<commit_message>
Add tests for electronics page
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testData.xlsx
+++ b/src/test/java/resources/testData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="78">
   <si>
     <t>Colombo</t>
   </si>
@@ -235,6 +236,30 @@
   </si>
   <si>
     <t>laptop</t>
+  </si>
+  <si>
+    <t>date_desc</t>
+  </si>
+  <si>
+    <t>Date: Newest on top</t>
+  </si>
+  <si>
+    <t>date_asc</t>
+  </si>
+  <si>
+    <t>Date: Oldest on top</t>
+  </si>
+  <si>
+    <t>price_desc</t>
+  </si>
+  <si>
+    <t>Price: High to low</t>
+  </si>
+  <si>
+    <t>price_asc</t>
+  </si>
+  <si>
+    <t>Price: Low to high</t>
   </si>
 </sst>
 </file>
@@ -569,7 +594,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C18" sqref="C1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -948,4 +973,266 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update tests for mobile phone page
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testData.xlsx
+++ b/src/test/java/resources/testData.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="96">
   <si>
     <t>Colombo</t>
   </si>
@@ -260,13 +261,67 @@
   </si>
   <si>
     <t>Price: Low to high</t>
+  </si>
+  <si>
+    <t>For Sale</t>
+  </si>
+  <si>
+    <t>Wanted</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Xiaomi</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Vivo</t>
+  </si>
+  <si>
+    <t>Galaxy S10</t>
+  </si>
+  <si>
+    <t>Galaxy A15</t>
+  </si>
+  <si>
+    <t>Redmi Note 13</t>
+  </si>
+  <si>
+    <t>Pixel 7 Pro</t>
+  </si>
+  <si>
+    <t>Pixel 5</t>
+  </si>
+  <si>
+    <t>Y93</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>iPhone 12 Pro</t>
+  </si>
+  <si>
+    <t>iPhone 11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +340,12 @@
       <color rgb="FF1D1B20"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -307,10 +368,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
@@ -1235,4 +1297,243 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1">
+        <v>100000</v>
+      </c>
+      <c r="F1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2">
+        <v>90000</v>
+      </c>
+      <c r="F2">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3">
+        <v>50000</v>
+      </c>
+      <c r="F3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5">
+        <v>30000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7">
+        <v>100000</v>
+      </c>
+      <c r="F7">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9">
+        <v>40000</v>
+      </c>
+      <c r="F9">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10">
+        <v>40000</v>
+      </c>
+      <c r="F10">
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test cases for property page
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testData.xlsx
+++ b/src/test/java/resources/testData.xlsx
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="108">
   <si>
     <t>Colombo</t>
   </si>
@@ -197,9 +200,6 @@
     <t>Services</t>
   </si>
   <si>
-    <t>Business &amp; Industry</t>
-  </si>
-  <si>
     <t>Nuwara Eliya</t>
   </si>
   <si>
@@ -315,6 +315,45 @@
   </si>
   <si>
     <t>iPhone 11</t>
+  </si>
+  <si>
+    <t>Monitor,Software,POS</t>
+  </si>
+  <si>
+    <t>RAM,Mouse,Keyboard,POS</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>DELL,ASUS,Kingston</t>
+  </si>
+  <si>
+    <t>Huawei</t>
+  </si>
+  <si>
+    <t>HP,Apple,TSC,EPSON</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>1,10</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>5,6,7</t>
+  </si>
+  <si>
+    <t>8,9,10</t>
   </si>
 </sst>
 </file>
@@ -655,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C1:C18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,7 +773,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>30</v>
@@ -778,7 +817,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>34</v>
@@ -839,7 +878,7 @@
         <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -850,7 +889,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -861,7 +900,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -877,7 +916,7 @@
     </row>
     <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>43</v>
@@ -949,7 +988,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -984,52 +1023,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1039,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,10 +1093,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
         <v>70</v>
-      </c>
-      <c r="B1" t="s">
-        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>51</v>
@@ -1065,10 +1104,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
         <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>51</v>
@@ -1076,10 +1115,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
         <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>51</v>
@@ -1087,10 +1126,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
         <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>51</v>
@@ -1098,10 +1137,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
         <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>52</v>
@@ -1109,10 +1148,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
         <v>72</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>52</v>
@@ -1120,10 +1159,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
         <v>74</v>
-      </c>
-      <c r="B7" t="s">
-        <v>75</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>52</v>
@@ -1131,10 +1170,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
         <v>76</v>
-      </c>
-      <c r="B8" t="s">
-        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>52</v>
@@ -1142,10 +1181,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
         <v>70</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>53</v>
@@ -1153,10 +1192,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
         <v>72</v>
-      </c>
-      <c r="B10" t="s">
-        <v>73</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>53</v>
@@ -1164,10 +1203,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
         <v>74</v>
-      </c>
-      <c r="B11" t="s">
-        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>53</v>
@@ -1175,10 +1214,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
         <v>76</v>
-      </c>
-      <c r="B12" t="s">
-        <v>77</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>53</v>
@@ -1186,10 +1225,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
         <v>70</v>
-      </c>
-      <c r="B13" t="s">
-        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -1197,10 +1236,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
         <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>54</v>
@@ -1208,10 +1247,10 @@
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
         <v>74</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>54</v>
@@ -1219,10 +1258,10 @@
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
         <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
@@ -1230,10 +1269,10 @@
     </row>
     <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
         <v>70</v>
-      </c>
-      <c r="B17" t="s">
-        <v>71</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>55</v>
@@ -1241,57 +1280,13 @@
     </row>
     <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
         <v>72</v>
-      </c>
-      <c r="B18" t="s">
-        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1303,7 +1298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -1314,16 +1309,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1">
         <v>100000</v>
@@ -1334,16 +1329,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2">
         <v>90000</v>
@@ -1354,16 +1349,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3">
         <v>50000</v>
@@ -1374,19 +1369,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4">
         <v>130000</v>
@@ -1394,56 +1389,56 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5">
         <v>30000</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7">
         <v>100000</v>
@@ -1454,36 +1449,36 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
         <v>91</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
       </c>
       <c r="E9">
         <v>40000</v>
@@ -1494,16 +1489,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10">
         <v>40000</v>
@@ -1514,26 +1509,435 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="25.77734375" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1">
+        <v>10000</v>
+      </c>
+      <c r="D1">
+        <v>50000</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2">
+        <v>20000</v>
+      </c>
+      <c r="D2">
+        <v>100000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3">
+        <v>30000</v>
+      </c>
+      <c r="D3">
+        <v>150000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+      <c r="D4">
+        <v>200000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6">
+        <v>15000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1">
+        <v>10000</v>
+      </c>
+      <c r="C1">
+        <v>50000</v>
+      </c>
+      <c r="D1">
+        <v>1000</v>
+      </c>
+      <c r="E1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2">
+        <v>20000</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>30000</v>
+      </c>
+      <c r="C3">
+        <v>150000</v>
+      </c>
+      <c r="D3">
+        <v>500</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>15000</v>
+      </c>
+      <c r="C4">
+        <v>200000</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6">
+        <v>15000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6">
+        <v>3000</v>
+      </c>
+      <c r="E6">
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1">
+        <v>10000</v>
+      </c>
+      <c r="C1">
+        <v>50000</v>
+      </c>
+      <c r="D1">
+        <v>1000</v>
+      </c>
+      <c r="E1">
+        <v>5000</v>
+      </c>
+      <c r="F1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2">
+        <v>20000</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2">
+        <v>2000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>30000</v>
+      </c>
+      <c r="C3">
+        <v>150000</v>
+      </c>
+      <c r="D3">
+        <v>500</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>15000</v>
+      </c>
+      <c r="C4">
+        <v>200000</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6">
+        <v>15000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6">
+        <v>3000</v>
+      </c>
+      <c r="E6">
+        <v>100000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add tests for vehicle pages
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testData.xlsx
+++ b/src/test/java/resources/testData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="135">
   <si>
     <t>Colombo</t>
   </si>
@@ -197,9 +199,6 @@
     <t>Home &amp; Garden</t>
   </si>
   <si>
-    <t>Services</t>
-  </si>
-  <si>
     <t>Nuwara Eliya</t>
   </si>
   <si>
@@ -354,13 +353,97 @@
   </si>
   <si>
     <t>8,9,10</t>
+  </si>
+  <si>
+    <t>reconditioned</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>Car Audio Systems,Bumper</t>
+  </si>
+  <si>
+    <t>Engines &amp; Engine Parts</t>
+  </si>
+  <si>
+    <t>Head Light,Tail Light,Doors</t>
+  </si>
+  <si>
+    <t>Lighting &amp; Indicators</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Suzuki</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Prius</t>
+  </si>
+  <si>
+    <t>Vezel</t>
+  </si>
+  <si>
+    <t>Wagon R</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>Motorbikes</t>
+  </si>
+  <si>
+    <t>Scooters</t>
+  </si>
+  <si>
+    <t>E-bikes</t>
+  </si>
+  <si>
+    <t>Quadricycles</t>
+  </si>
+  <si>
+    <t>Bajaj</t>
+  </si>
+  <si>
+    <t>Hero</t>
+  </si>
+  <si>
+    <t>Yamaha</t>
+  </si>
+  <si>
+    <t>TVS</t>
+  </si>
+  <si>
+    <t>CT100</t>
+  </si>
+  <si>
+    <t>CB Shine</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>Zest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,6 +469,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1B20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -407,11 +497,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,7 +865,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>30</v>
@@ -817,7 +909,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>34</v>
@@ -845,7 +937,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -856,7 +948,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -867,7 +959,7 @@
         <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -916,7 +1008,7 @@
     </row>
     <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>43</v>
@@ -988,7 +1080,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -999,7 +1091,7 @@
         <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1023,52 +1115,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1078,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1093,10 +1185,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" t="s">
-        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>51</v>
@@ -1104,10 +1196,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>51</v>
@@ -1115,10 +1207,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
         <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>51</v>
@@ -1126,10 +1218,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>51</v>
@@ -1137,10 +1229,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
         <v>69</v>
-      </c>
-      <c r="B5" t="s">
-        <v>70</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>52</v>
@@ -1148,10 +1240,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>71</v>
-      </c>
-      <c r="B6" t="s">
-        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>52</v>
@@ -1159,10 +1251,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
         <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>52</v>
@@ -1170,10 +1262,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
         <v>75</v>
-      </c>
-      <c r="B8" t="s">
-        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>52</v>
@@ -1181,10 +1273,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
         <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>70</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>53</v>
@@ -1192,10 +1284,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
         <v>71</v>
-      </c>
-      <c r="B10" t="s">
-        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>53</v>
@@ -1203,10 +1295,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
         <v>73</v>
-      </c>
-      <c r="B11" t="s">
-        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>53</v>
@@ -1214,10 +1306,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
         <v>75</v>
-      </c>
-      <c r="B12" t="s">
-        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>53</v>
@@ -1225,10 +1317,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
         <v>69</v>
-      </c>
-      <c r="B13" t="s">
-        <v>70</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -1236,10 +1328,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
         <v>71</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>54</v>
@@ -1247,10 +1339,10 @@
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>54</v>
@@ -1258,35 +1350,13 @@
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
         <v>75</v>
-      </c>
-      <c r="B16" t="s">
-        <v>76</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1309,16 +1379,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1">
         <v>100000</v>
@@ -1329,16 +1399,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2">
         <v>90000</v>
@@ -1349,16 +1419,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3">
         <v>50000</v>
@@ -1369,19 +1439,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4">
         <v>130000</v>
@@ -1389,56 +1459,56 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5">
         <v>30000</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7">
         <v>100000</v>
@@ -1449,36 +1519,36 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
         <v>90</v>
-      </c>
-      <c r="D9" t="s">
-        <v>91</v>
       </c>
       <c r="E9">
         <v>40000</v>
@@ -1489,16 +1559,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10">
         <v>40000</v>
@@ -1509,22 +1579,22 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1549,10 +1619,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1">
         <v>10000</v>
@@ -1561,18 +1631,18 @@
         <v>50000</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2">
         <v>20000</v>
@@ -1581,18 +1651,18 @@
         <v>100000</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3">
         <v>30000</v>
@@ -1601,18 +1671,18 @@
         <v>150000</v>
       </c>
       <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
         <v>97</v>
-      </c>
-      <c r="F3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4">
         <v>15000</v>
@@ -1621,50 +1691,50 @@
         <v>200000</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6">
         <v>15000</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
         <v>101</v>
-      </c>
-      <c r="F6" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1677,14 +1747,14 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E6"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1">
         <v>10000</v>
@@ -1701,7 +1771,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2">
         <v>20000</v>
@@ -1710,7 +1780,7 @@
         <v>100000</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2">
         <v>2000</v>
@@ -1718,7 +1788,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3">
         <v>30000</v>
@@ -1730,12 +1800,12 @@
         <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -1752,30 +1822,30 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6">
         <v>15000</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6">
         <v>3000</v>
@@ -1794,14 +1864,14 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B1" sqref="B1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1">
         <v>10000</v>
@@ -1816,15 +1886,15 @@
         <v>5000</v>
       </c>
       <c r="F1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" t="s">
         <v>103</v>
-      </c>
-      <c r="G1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2">
         <v>20000</v>
@@ -1833,13 +1903,13 @@
         <v>100000</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2">
         <v>2000</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1847,7 +1917,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3">
         <v>30000</v>
@@ -1859,18 +1929,18 @@
         <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -1893,36 +1963,36 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6">
         <v>15000</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6">
         <v>3000</v>
@@ -1931,10 +2001,397 @@
         <v>100000</v>
       </c>
       <c r="F6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" t="s">
         <v>106</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="34.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1">
+        <v>10000</v>
+      </c>
+      <c r="D1">
+        <v>50000</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2">
+        <v>20000</v>
+      </c>
+      <c r="D2">
+        <v>100000</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3">
+        <v>30000</v>
+      </c>
+      <c r="D3">
+        <v>150000</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+      <c r="D4">
+        <v>200000</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6">
+        <v>15000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1">
+        <v>10000</v>
+      </c>
+      <c r="E1">
+        <v>50000</v>
+      </c>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1">
+        <v>2019</v>
+      </c>
+      <c r="I1">
+        <v>2022</v>
+      </c>
+      <c r="J1">
+        <v>40000</v>
+      </c>
+      <c r="K1">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2">
+        <v>20000</v>
+      </c>
+      <c r="E2">
+        <v>100000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2">
+        <v>2019</v>
+      </c>
+      <c r="J2">
+        <v>30000</v>
+      </c>
+      <c r="K2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3">
+        <v>30000</v>
+      </c>
+      <c r="E3">
+        <v>150000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3">
+        <v>2023</v>
+      </c>
+      <c r="I3">
+        <v>2024</v>
+      </c>
+      <c r="J3">
+        <v>20000</v>
+      </c>
+      <c r="K3">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4">
+        <v>15000</v>
+      </c>
+      <c r="E4">
+        <v>200000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4">
+        <v>2010</v>
+      </c>
+      <c r="I4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>15000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>130</v>
+      </c>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>134</v>
+      </c>
+      <c r="H6">
+        <v>2015</v>
+      </c>
+      <c r="I6">
+        <v>2015</v>
+      </c>
+      <c r="J6">
+        <v>5000</v>
+      </c>
+      <c r="K6">
+        <v>25000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add home and garden page releated tests
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testData.xlsx
+++ b/src/test/java/resources/testData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="143">
   <si>
     <t>Colombo</t>
   </si>
@@ -437,6 +438,30 @@
   </si>
   <si>
     <t>Zest</t>
+  </si>
+  <si>
+    <t>Living Room Furniture</t>
+  </si>
+  <si>
+    <t>Shelves &amp; Pantry Cupboards</t>
+  </si>
+  <si>
+    <t>Bedroom Furniture,Shelves &amp; Pantry Cupboards</t>
+  </si>
+  <si>
+    <t>Tables &amp; Chairs,Lighting,Textiles / decoration</t>
+  </si>
+  <si>
+    <t>Arpico</t>
+  </si>
+  <si>
+    <t>E H Cooray,Softlogic</t>
+  </si>
+  <si>
+    <t>Nilkamal,Don Corolis,Nisako</t>
+  </si>
+  <si>
+    <t>Nippon</t>
   </si>
 </sst>
 </file>
@@ -1100,12 +1125,152 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="49.109375" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1">
+        <v>10000</v>
+      </c>
+      <c r="D1">
+        <v>50000</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2">
+        <v>20000</v>
+      </c>
+      <c r="D2">
+        <v>100000</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3">
+        <v>30000</v>
+      </c>
+      <c r="D3">
+        <v>150000</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+      <c r="D4">
+        <v>200000</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6">
+        <v>15000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -1608,7 +1773,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D6"/>
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1747,7 +1912,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1864,7 +2029,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C6"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>